<commit_message>
Refactored to and from xlsx to use only a mapping for an entry id.
</commit_message>
<xml_diff>
--- a/tests/io/data/expected-load-file.xlsx
+++ b/tests/io/data/expected-load-file.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="test_dict" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="__footings__" sheetId="2" state="hidden" r:id="rId2"/>
+    <sheet name="test_dict" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="__footings__" sheetId="2" state="hidden" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -473,7 +473,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -489,50 +489,30 @@
       </c>
       <c r="B1" t="inlineStr">
         <is>
-          <t>source</t>
+          <t>mapping</t>
         </is>
       </c>
       <c r="C1" t="inlineStr">
         <is>
-          <t>mapping</t>
+          <t>dtype</t>
         </is>
       </c>
       <c r="D1" t="inlineStr">
         <is>
-          <t>end_point</t>
+          <t>row_start</t>
         </is>
       </c>
       <c r="E1" t="inlineStr">
         <is>
-          <t>column_name</t>
+          <t>col_start</t>
         </is>
       </c>
       <c r="F1" t="inlineStr">
         <is>
-          <t>dtype</t>
+          <t>row_end</t>
         </is>
       </c>
       <c r="G1" t="inlineStr">
-        <is>
-          <t>stable</t>
-        </is>
-      </c>
-      <c r="H1" t="inlineStr">
-        <is>
-          <t>row_start</t>
-        </is>
-      </c>
-      <c r="I1" t="inlineStr">
-        <is>
-          <t>col_start</t>
-        </is>
-      </c>
-      <c r="J1" t="inlineStr">
-        <is>
-          <t>row_end</t>
-        </is>
-      </c>
-      <c r="K1" t="inlineStr">
         <is>
           <t>col_end</t>
         </is>
@@ -544,31 +524,26 @@
           <t>test_dict</t>
         </is>
       </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>/outer</t>
+        </is>
+      </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>/outer/</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>KEY</t>
-        </is>
-      </c>
-      <c r="F2" t="inlineStr">
-        <is>
           <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
-      <c r="H2" t="n">
-        <v>2</v>
-      </c>
-      <c r="I2" t="n">
-        <v>2</v>
-      </c>
-      <c r="J2" t="n">
-        <v>2</v>
-      </c>
-      <c r="K2" t="n">
+      <c r="D2" t="n">
+        <v>2</v>
+      </c>
+      <c r="E2" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" t="n">
+        <v>2</v>
+      </c>
+      <c r="G2" t="n">
         <v>2</v>
       </c>
     </row>
@@ -578,31 +553,26 @@
           <t>test_dict</t>
         </is>
       </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>/outer/inner</t>
+        </is>
+      </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>/outer/inner/</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>KEY</t>
-        </is>
-      </c>
-      <c r="F3" t="inlineStr">
-        <is>
           <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
-      <c r="H3" t="n">
-        <v>2</v>
-      </c>
-      <c r="I3" t="n">
-        <v>3</v>
-      </c>
-      <c r="J3" t="n">
-        <v>2</v>
-      </c>
-      <c r="K3" t="n">
+      <c r="D3" t="n">
+        <v>2</v>
+      </c>
+      <c r="E3" t="n">
+        <v>3</v>
+      </c>
+      <c r="F3" t="n">
+        <v>2</v>
+      </c>
+      <c r="G3" t="n">
         <v>3</v>
       </c>
     </row>
@@ -612,31 +582,26 @@
           <t>test_dict</t>
         </is>
       </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>/outer/inner/endpoint1</t>
+        </is>
+      </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>/outer/inner/endpoint1/</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>KEY</t>
-        </is>
-      </c>
-      <c r="F4" t="inlineStr">
-        <is>
           <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
-      <c r="H4" t="n">
-        <v>2</v>
-      </c>
-      <c r="I4" t="n">
+      <c r="D4" t="n">
+        <v>2</v>
+      </c>
+      <c r="E4" t="n">
         <v>4</v>
       </c>
-      <c r="J4" t="n">
-        <v>2</v>
-      </c>
-      <c r="K4" t="n">
+      <c r="F4" t="n">
+        <v>2</v>
+      </c>
+      <c r="G4" t="n">
         <v>4</v>
       </c>
     </row>
@@ -646,31 +611,26 @@
           <t>test_dict</t>
         </is>
       </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>/outer/inner/endpoint1</t>
+        </is>
+      </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>/outer/inner/endpoint1/</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>VALUE</t>
-        </is>
-      </c>
-      <c r="F5" t="inlineStr">
-        <is>
           <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
-      <c r="H5" t="n">
-        <v>2</v>
-      </c>
-      <c r="I5" t="n">
+      <c r="D5" t="n">
+        <v>2</v>
+      </c>
+      <c r="E5" t="n">
         <v>5</v>
       </c>
-      <c r="J5" t="n">
-        <v>2</v>
-      </c>
-      <c r="K5" t="n">
+      <c r="F5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G5" t="n">
         <v>5</v>
       </c>
     </row>
@@ -680,31 +640,26 @@
           <t>test_dict</t>
         </is>
       </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>/outer/inner/endpoint2</t>
+        </is>
+      </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>/outer/inner/endpoint2/</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>KEY</t>
-        </is>
-      </c>
-      <c r="F6" t="inlineStr">
-        <is>
           <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
-      <c r="H6" t="n">
-        <v>3</v>
-      </c>
-      <c r="I6" t="n">
+      <c r="D6" t="n">
+        <v>3</v>
+      </c>
+      <c r="E6" t="n">
         <v>4</v>
       </c>
-      <c r="J6" t="n">
-        <v>3</v>
-      </c>
-      <c r="K6" t="n">
+      <c r="F6" t="n">
+        <v>3</v>
+      </c>
+      <c r="G6" t="n">
         <v>4</v>
       </c>
     </row>
@@ -714,31 +669,26 @@
           <t>test_dict</t>
         </is>
       </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>/outer/inner/endpoint2</t>
+        </is>
+      </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>/outer/inner/endpoint2/</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>VALUE</t>
-        </is>
-      </c>
-      <c r="F7" t="inlineStr">
-        <is>
           <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
-      <c r="H7" t="n">
-        <v>3</v>
-      </c>
-      <c r="I7" t="n">
+      <c r="D7" t="n">
+        <v>3</v>
+      </c>
+      <c r="E7" t="n">
         <v>5</v>
       </c>
-      <c r="J7" t="n">
-        <v>3</v>
-      </c>
-      <c r="K7" t="n">
+      <c r="F7" t="n">
+        <v>3</v>
+      </c>
+      <c r="G7" t="n">
         <v>5</v>
       </c>
     </row>
@@ -748,31 +698,26 @@
           <t>test_dict</t>
         </is>
       </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>/endpoint3</t>
+        </is>
+      </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>/endpoint3/</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>KEY</t>
-        </is>
-      </c>
-      <c r="F8" t="inlineStr">
-        <is>
           <t>&lt;class 'str'&gt;</t>
         </is>
       </c>
-      <c r="H8" t="n">
+      <c r="D8" t="n">
         <v>4</v>
       </c>
-      <c r="I8" t="n">
-        <v>2</v>
-      </c>
-      <c r="J8" t="n">
+      <c r="E8" t="n">
+        <v>2</v>
+      </c>
+      <c r="F8" t="n">
         <v>4</v>
       </c>
-      <c r="K8" t="n">
+      <c r="G8" t="n">
         <v>2</v>
       </c>
     </row>
@@ -782,31 +727,26 @@
           <t>test_dict</t>
         </is>
       </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>/endpoint3</t>
+        </is>
+      </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>/endpoint3/</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>VALUE</t>
-        </is>
-      </c>
-      <c r="F9" t="inlineStr">
-        <is>
           <t>&lt;class 'int'&gt;</t>
         </is>
       </c>
-      <c r="H9" t="n">
+      <c r="D9" t="n">
         <v>4</v>
       </c>
-      <c r="I9" t="n">
-        <v>3</v>
-      </c>
-      <c r="J9" t="n">
+      <c r="E9" t="n">
+        <v>3</v>
+      </c>
+      <c r="F9" t="n">
         <v>4</v>
       </c>
-      <c r="K9" t="n">
+      <c r="G9" t="n">
         <v>3</v>
       </c>
     </row>

</xml_diff>